<commit_message>
alteracoes na area de cadastro de ids dos alunos
</commit_message>
<xml_diff>
--- a/biblioteca.xlsx
+++ b/biblioteca.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Pojeto Biblioteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADEBD1F-DE72-4CF5-90EA-65FC6C389B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A353E37-65B1-46F4-9AEF-5BBD3D9BE2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2745" windowWidth="18015" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2745" windowWidth="18015" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alunos" sheetId="1" r:id="rId1"/>
@@ -410,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +422,7 @@
     <col min="7" max="7" width="45.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finalizando exportação de alterações de dados alunos/livros na planilha
</commit_message>
<xml_diff>
--- a/biblioteca.xlsx
+++ b/biblioteca.xlsx
@@ -1,83 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Pojeto Biblioteca\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A353E37-65B1-46F4-9AEF-5BBD3D9BE2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2745" windowWidth="18015" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5145" yWindow="2475" windowWidth="18015" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="alunos" sheetId="1" r:id="rId1"/>
-    <sheet name="livros" sheetId="2" r:id="rId2"/>
+    <sheet name="alunos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="livros" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>SERIE</t>
-  </si>
-  <si>
-    <t>TURNO</t>
-  </si>
-  <si>
-    <t>IDADE</t>
-  </si>
-  <si>
-    <t>CONTATO</t>
-  </si>
-  <si>
-    <t>ENDERECO</t>
-  </si>
-  <si>
-    <t>TITULO</t>
-  </si>
-  <si>
-    <t>GENERO</t>
-  </si>
-  <si>
-    <t>AUTOR</t>
-  </si>
-  <si>
-    <t>EDITORA</t>
-  </si>
-  <si>
-    <t>QUANTIDADE</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\(00\)\ 0\ 0000\-0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,30 +49,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -407,86 +419,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" style="2" customWidth="1"/>
+    <col width="12.140625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="36.42578125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="9.140625" customWidth="1" style="1" min="3" max="5"/>
+    <col width="18.140625" customWidth="1" style="3" min="6" max="6"/>
+    <col width="45.85546875" customWidth="1" style="2" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+    <row r="1" ht="16.5" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NOME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SERIE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>TURNO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IDADE</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>CONTATO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ENDERECO</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
+    <col width="11.85546875" customWidth="1" style="1" min="1" max="1"/>
+    <col width="32.85546875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="23.28515625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="12" customWidth="1" style="1" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>TITULO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>AUTOR</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EDITORA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>QUANTIDADE</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criando meu primeiro gitignore
</commit_message>
<xml_diff>
--- a/biblioteca.xlsx
+++ b/biblioteca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Projeto-Biblioteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C041E5-1FA7-42FB-92EA-1A04260936A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342435E-5151-45F0-83E9-A2B6E1265CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="2475" windowWidth="18015" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>QUANTIDADE</t>
-  </si>
-  <si>
-    <t>wellington</t>
-  </si>
-  <si>
-    <t>teste</t>
   </si>
 </sst>
 </file>
@@ -460,10 +454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,17 +490,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>123</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
implementando mecanismos de buscas especificas nas aréas de emprestimo e desvolução de livros
</commit_message>
<xml_diff>
--- a/biblioteca.xlsx
+++ b/biblioteca.xlsx
@@ -1,96 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Projeto-Biblioteca\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5ECFB-B73C-401E-9DA9-27F56CA204C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="2820" windowWidth="18015" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5490" yWindow="2820" windowWidth="18015" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="alunos" sheetId="1" r:id="rId1"/>
-    <sheet name="livros" sheetId="2" r:id="rId2"/>
-    <sheet name="emprestimos" sheetId="3" r:id="rId3"/>
+    <sheet name="alunos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="livros" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="emprestimos" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>SERIE</t>
-  </si>
-  <si>
-    <t>TURNO</t>
-  </si>
-  <si>
-    <t>IDADE</t>
-  </si>
-  <si>
-    <t>CONTATO</t>
-  </si>
-  <si>
-    <t>ENDERECO</t>
-  </si>
-  <si>
-    <t>TITULO</t>
-  </si>
-  <si>
-    <t>GENERO</t>
-  </si>
-  <si>
-    <t>AUTOR</t>
-  </si>
-  <si>
-    <t>EDITORA</t>
-  </si>
-  <si>
-    <t>QUANTIDADE</t>
-  </si>
-  <si>
-    <t>ID EMPRESTIMO</t>
-  </si>
-  <si>
-    <t>INFORMACOES ALUNO</t>
-  </si>
-  <si>
-    <t>LIVRO</t>
-  </si>
-  <si>
-    <t>DEVOLUCAO</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\(00\)\ 0\ 0000\-0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -109,30 +50,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,87 +420,332 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12.140625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="36.42578125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="9.140625" customWidth="1" style="1" min="3" max="5"/>
+    <col width="18.140625" customWidth="1" style="3" min="6" max="6"/>
+    <col width="45.85546875" customWidth="1" style="2" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.5" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NOME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SERIE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>TURNO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IDADE</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>CONTATO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ENDERECO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>wellington</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>tarde</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>rua1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>dandan</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tarde </t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>rua2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>daniel</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>7 manha</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>rua3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pedin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Manha</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>19</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>90898948</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Rua 687</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Aquila</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>99</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0989</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Granvile</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pednhiriq</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>79</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>723283</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" style="2" customWidth="1"/>
+    <col width="11.85546875" customWidth="1" style="1" min="1" max="1"/>
+    <col width="32.85546875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="23.28515625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="12" customWidth="1" style="1" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" style="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>TITULO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GENERO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>AUTOR</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EDITORA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>QUANTIDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>123</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Sei la</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Terror</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Eu</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sal</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -509,38 +754,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="63.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="1" customWidth="1"/>
+    <col width="16.42578125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="63.140625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="28.140625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="20.140625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="17" customWidth="1" style="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID EMPRESTIMO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>INFORMACOES ALUNO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LIVRO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>DEVOLUCAO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>31212</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[3, 'daniel', '7 manha', None, 18, 3, 'rua3']</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>o todo poderoso</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12/12</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" customFormat="1" s="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>31312</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>[3, 'daniel', '7 manha', None, 18, 3, 'rua3']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sei nao</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>13/12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alguns testes na planilha
</commit_message>
<xml_diff>
--- a/biblioteca.xlsx
+++ b/biblioteca.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5490" yWindow="2820" windowWidth="18015" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="alunos" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="livros" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="emprestimos" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="alunos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="livros" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="emprestimos" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -425,13 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="36.42578125" customWidth="1" style="1" min="2" max="2"/>
@@ -657,6 +657,72 @@
       <c r="G7" t="inlineStr">
         <is>
           <t>Jose</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Wellington almeida</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>7 ani</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>88 9 81762299</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Rua 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rian</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>9 ano</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>20</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>88 99 99 99999</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Rua 3</t>
         </is>
       </c>
     </row>
@@ -678,7 +744,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="11.85546875" customWidth="1" style="1" min="1" max="1"/>
     <col width="32.85546875" customWidth="1" style="1" min="2" max="2"/>
@@ -759,13 +825,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="16.42578125" customWidth="1" style="1" min="1" max="1"/>
     <col width="63.140625" customWidth="1" style="1" min="2" max="2"/>
@@ -818,28 +884,7 @@
         </is>
       </c>
     </row>
-    <row r="3" customFormat="1" s="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>31312</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>[3, 'daniel', '7 manha', None, 18, 3, 'rua3']</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>sei nao</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>13/12</t>
-        </is>
-      </c>
-    </row>
+    <row r="3" customFormat="1" s="1"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>